<commit_message>
load_condition_from excel function with nodes pressures
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/ConditionsWithP.xlsx
+++ b/eureca_dhcs/test/input_tests/ConditionsWithP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\OneDrive - Università degli Studi di Padova\AttivitaDavis\MeteredData\AnalysisCoolingNetwork\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\Desktop\eureca-dhcs\eureca_dhcs\test\input_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_D92097028173A5C1A0E926406918EDE8E7C12B4B" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{89354C0A-986B-466C-BE7E-906148045345}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C00E869-3608-47ED-BF13-DF35B7506F60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="0" windowWidth="16560" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2808" yWindow="0" windowWidth="16560" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
   <dimension ref="A1:T339"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q2"/>
+      <selection activeCell="R2" sqref="R2:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
removed exception for mass flow rate not given
</commit_message>
<xml_diff>
--- a/eureca_dhcs/test/input_tests/ConditionsWithP.xlsx
+++ b/eureca_dhcs/test/input_tests/ConditionsWithP.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratenr15640\Desktop\eureca-dhcs\eureca_dhcs\test\input_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C00E869-3608-47ED-BF13-DF35B7506F60}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A2C77E-88E0-48D7-8407-B353B4B20BD7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2808" yWindow="0" windowWidth="16560" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3744" yWindow="0" windowWidth="16560" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydraulic" sheetId="1" r:id="rId1"/>
+    <sheet name="Thermal" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
   <si>
     <t>Node</t>
   </si>
@@ -29,6 +30,9 @@
   </si>
   <si>
     <t>Pressure [Pa]</t>
+  </si>
+  <si>
+    <t>Temperature [°C]</t>
   </si>
 </sst>
 </file>
@@ -124,12 +128,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -448,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T339"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2:T2"/>
+    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
+      <selection activeCell="D326" sqref="D326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,53 +466,53 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="3" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -21407,4 +21414,4755 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9C73D5-1E36-497D-9821-E44B325038FE}">
+  <dimension ref="A1:D339"/>
+  <sheetViews>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3">
+        <v>119</v>
+      </c>
+      <c r="C3" s="3">
+        <v>95</v>
+      </c>
+      <c r="D3" s="3">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>44363</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>44363.041666666657</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>44363.083333333343</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>44363.125</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>44363.166666666657</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>44363.208333333343</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>44363.25</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>44363.291666666657</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>44363.333333333343</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>44363.375</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>44363.416666666657</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>44363.458333333343</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>44363.5</v>
+      </c>
+      <c r="B16">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>44363.541666666657</v>
+      </c>
+      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>44363.583333333343</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>44363.625</v>
+      </c>
+      <c r="B19">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>44363.666666666657</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>44363.708333333343</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>44363.75</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>44363.791666666657</v>
+      </c>
+      <c r="B23">
+        <v>10</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>44363.833333333343</v>
+      </c>
+      <c r="B24">
+        <v>10</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>44363.875</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>44363.916666666657</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>44363.958333333343</v>
+      </c>
+      <c r="B27">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>10</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>44364</v>
+      </c>
+      <c r="B28">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>44364.041666666657</v>
+      </c>
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>44364.083333333343</v>
+      </c>
+      <c r="B30">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>44364.125</v>
+      </c>
+      <c r="B31">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>44364.166666666657</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>10</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>44364.208333333343</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>44364.25</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>44364.291666666657</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>10</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>44364.333333333343</v>
+      </c>
+      <c r="B36">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>44364.375</v>
+      </c>
+      <c r="B37">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>10</v>
+      </c>
+      <c r="D37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>44364.416666666657</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>44364.458333333343</v>
+      </c>
+      <c r="B39">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>10</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>44364.5</v>
+      </c>
+      <c r="B40">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>44364.541666666657</v>
+      </c>
+      <c r="B41">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>44364.583333333343</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>44364.625</v>
+      </c>
+      <c r="B43">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>44364.666666666657</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>44364.708333333343</v>
+      </c>
+      <c r="B45">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>44364.75</v>
+      </c>
+      <c r="B46">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>44364.791666666657</v>
+      </c>
+      <c r="B47">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>44364.833333333343</v>
+      </c>
+      <c r="B48">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>44364.875</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>44364.916666666657</v>
+      </c>
+      <c r="B50">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>44364.958333333343</v>
+      </c>
+      <c r="B51">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>44365</v>
+      </c>
+      <c r="B52">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>44365.041666666657</v>
+      </c>
+      <c r="B53">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>44365.083333333343</v>
+      </c>
+      <c r="B54">
+        <v>10</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>44365.125</v>
+      </c>
+      <c r="B55">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>44365.166666666657</v>
+      </c>
+      <c r="B56">
+        <v>10</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
+      </c>
+      <c r="D56">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>44365.208333333343</v>
+      </c>
+      <c r="B57">
+        <v>10</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
+      </c>
+      <c r="D57">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>44365.25</v>
+      </c>
+      <c r="B58">
+        <v>10</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="D58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>44365.291666666657</v>
+      </c>
+      <c r="B59">
+        <v>10</v>
+      </c>
+      <c r="C59">
+        <v>10</v>
+      </c>
+      <c r="D59">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>44365.333333333343</v>
+      </c>
+      <c r="B60">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>44365.375</v>
+      </c>
+      <c r="B61">
+        <v>10</v>
+      </c>
+      <c r="C61">
+        <v>10</v>
+      </c>
+      <c r="D61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>44365.416666666657</v>
+      </c>
+      <c r="B62">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>10</v>
+      </c>
+      <c r="D62">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>44365.458333333343</v>
+      </c>
+      <c r="B63">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>10</v>
+      </c>
+      <c r="D63">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>44365.5</v>
+      </c>
+      <c r="B64">
+        <v>10</v>
+      </c>
+      <c r="C64">
+        <v>10</v>
+      </c>
+      <c r="D64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>44365.541666666657</v>
+      </c>
+      <c r="B65">
+        <v>10</v>
+      </c>
+      <c r="C65">
+        <v>10</v>
+      </c>
+      <c r="D65">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>44365.583333333343</v>
+      </c>
+      <c r="B66">
+        <v>10</v>
+      </c>
+      <c r="C66">
+        <v>10</v>
+      </c>
+      <c r="D66">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>44365.625</v>
+      </c>
+      <c r="B67">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="D67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>44365.666666666657</v>
+      </c>
+      <c r="B68">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>10</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>44365.708333333343</v>
+      </c>
+      <c r="B69">
+        <v>10</v>
+      </c>
+      <c r="C69">
+        <v>10</v>
+      </c>
+      <c r="D69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>44365.75</v>
+      </c>
+      <c r="B70">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <v>10</v>
+      </c>
+      <c r="D70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>44365.791666666657</v>
+      </c>
+      <c r="B71">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>10</v>
+      </c>
+      <c r="D71">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>44365.833333333343</v>
+      </c>
+      <c r="B72">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>10</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>44365.875</v>
+      </c>
+      <c r="B73">
+        <v>10</v>
+      </c>
+      <c r="C73">
+        <v>10</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="2">
+        <v>44365.916666666657</v>
+      </c>
+      <c r="B74">
+        <v>10</v>
+      </c>
+      <c r="C74">
+        <v>10</v>
+      </c>
+      <c r="D74">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="2">
+        <v>44365.958333333343</v>
+      </c>
+      <c r="B75">
+        <v>10</v>
+      </c>
+      <c r="C75">
+        <v>10</v>
+      </c>
+      <c r="D75">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="2">
+        <v>44366</v>
+      </c>
+      <c r="B76">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <v>10</v>
+      </c>
+      <c r="D76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" s="2">
+        <v>44366.041666666657</v>
+      </c>
+      <c r="B77">
+        <v>10</v>
+      </c>
+      <c r="C77">
+        <v>10</v>
+      </c>
+      <c r="D77">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="2">
+        <v>44366.083333333343</v>
+      </c>
+      <c r="B78">
+        <v>10</v>
+      </c>
+      <c r="C78">
+        <v>10</v>
+      </c>
+      <c r="D78">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="2">
+        <v>44366.125</v>
+      </c>
+      <c r="B79">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>10</v>
+      </c>
+      <c r="D79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="2">
+        <v>44366.166666666657</v>
+      </c>
+      <c r="B80">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>10</v>
+      </c>
+      <c r="D80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="2">
+        <v>44366.208333333343</v>
+      </c>
+      <c r="B81">
+        <v>10</v>
+      </c>
+      <c r="C81">
+        <v>10</v>
+      </c>
+      <c r="D81">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="2">
+        <v>44366.25</v>
+      </c>
+      <c r="B82">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="2">
+        <v>44366.291666666657</v>
+      </c>
+      <c r="B83">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>10</v>
+      </c>
+      <c r="D83">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="2">
+        <v>44366.333333333343</v>
+      </c>
+      <c r="B84">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>10</v>
+      </c>
+      <c r="D84">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="2">
+        <v>44366.375</v>
+      </c>
+      <c r="B85">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>10</v>
+      </c>
+      <c r="D85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="2">
+        <v>44366.416666666657</v>
+      </c>
+      <c r="B86">
+        <v>10</v>
+      </c>
+      <c r="C86">
+        <v>10</v>
+      </c>
+      <c r="D86">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="2">
+        <v>44366.458333333343</v>
+      </c>
+      <c r="B87">
+        <v>10</v>
+      </c>
+      <c r="C87">
+        <v>10</v>
+      </c>
+      <c r="D87">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="2">
+        <v>44366.5</v>
+      </c>
+      <c r="B88">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>10</v>
+      </c>
+      <c r="D88">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="2">
+        <v>44366.541666666657</v>
+      </c>
+      <c r="B89">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>10</v>
+      </c>
+      <c r="D89">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="2">
+        <v>44366.583333333343</v>
+      </c>
+      <c r="B90">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>10</v>
+      </c>
+      <c r="D90">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="2">
+        <v>44366.625</v>
+      </c>
+      <c r="B91">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>10</v>
+      </c>
+      <c r="D91">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="2">
+        <v>44366.666666666657</v>
+      </c>
+      <c r="B92">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="2">
+        <v>44366.708333333343</v>
+      </c>
+      <c r="B93">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>10</v>
+      </c>
+      <c r="D93">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="2">
+        <v>44366.75</v>
+      </c>
+      <c r="B94">
+        <v>10</v>
+      </c>
+      <c r="C94">
+        <v>10</v>
+      </c>
+      <c r="D94">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="2">
+        <v>44366.791666666657</v>
+      </c>
+      <c r="B95">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>10</v>
+      </c>
+      <c r="D95">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="2">
+        <v>44366.833333333343</v>
+      </c>
+      <c r="B96">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>10</v>
+      </c>
+      <c r="D96">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="2">
+        <v>44366.875</v>
+      </c>
+      <c r="B97">
+        <v>10</v>
+      </c>
+      <c r="C97">
+        <v>10</v>
+      </c>
+      <c r="D97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="2">
+        <v>44366.916666666657</v>
+      </c>
+      <c r="B98">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>10</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" s="2">
+        <v>44366.958333333343</v>
+      </c>
+      <c r="B99">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>10</v>
+      </c>
+      <c r="D99">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="2">
+        <v>44367</v>
+      </c>
+      <c r="B100">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>10</v>
+      </c>
+      <c r="D100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="2">
+        <v>44367.041666666657</v>
+      </c>
+      <c r="B101">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>10</v>
+      </c>
+      <c r="D101">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="2">
+        <v>44367.083333333343</v>
+      </c>
+      <c r="B102">
+        <v>10</v>
+      </c>
+      <c r="C102">
+        <v>10</v>
+      </c>
+      <c r="D102">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="2">
+        <v>44367.125</v>
+      </c>
+      <c r="B103">
+        <v>10</v>
+      </c>
+      <c r="C103">
+        <v>10</v>
+      </c>
+      <c r="D103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="2">
+        <v>44367.166666666657</v>
+      </c>
+      <c r="B104">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>10</v>
+      </c>
+      <c r="D104">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="2">
+        <v>44367.208333333343</v>
+      </c>
+      <c r="B105">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>10</v>
+      </c>
+      <c r="D105">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="2">
+        <v>44367.25</v>
+      </c>
+      <c r="B106">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>10</v>
+      </c>
+      <c r="D106">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="2">
+        <v>44367.291666666657</v>
+      </c>
+      <c r="B107">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>10</v>
+      </c>
+      <c r="D107">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="2">
+        <v>44367.333333333343</v>
+      </c>
+      <c r="B108">
+        <v>10</v>
+      </c>
+      <c r="C108">
+        <v>10</v>
+      </c>
+      <c r="D108">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="2">
+        <v>44367.375</v>
+      </c>
+      <c r="B109">
+        <v>10</v>
+      </c>
+      <c r="C109">
+        <v>10</v>
+      </c>
+      <c r="D109">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" s="2">
+        <v>44367.416666666657</v>
+      </c>
+      <c r="B110">
+        <v>10</v>
+      </c>
+      <c r="C110">
+        <v>10</v>
+      </c>
+      <c r="D110">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" s="2">
+        <v>44367.458333333343</v>
+      </c>
+      <c r="B111">
+        <v>10</v>
+      </c>
+      <c r="C111">
+        <v>10</v>
+      </c>
+      <c r="D111">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="2">
+        <v>44367.5</v>
+      </c>
+      <c r="B112">
+        <v>10</v>
+      </c>
+      <c r="C112">
+        <v>10</v>
+      </c>
+      <c r="D112">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="2">
+        <v>44367.541666666657</v>
+      </c>
+      <c r="B113">
+        <v>10</v>
+      </c>
+      <c r="C113">
+        <v>10</v>
+      </c>
+      <c r="D113">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="2">
+        <v>44367.583333333343</v>
+      </c>
+      <c r="B114">
+        <v>10</v>
+      </c>
+      <c r="C114">
+        <v>10</v>
+      </c>
+      <c r="D114">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="2">
+        <v>44367.625</v>
+      </c>
+      <c r="B115">
+        <v>10</v>
+      </c>
+      <c r="C115">
+        <v>10</v>
+      </c>
+      <c r="D115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="2">
+        <v>44367.666666666657</v>
+      </c>
+      <c r="B116">
+        <v>10</v>
+      </c>
+      <c r="C116">
+        <v>10</v>
+      </c>
+      <c r="D116">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="2">
+        <v>44367.708333333343</v>
+      </c>
+      <c r="B117">
+        <v>10</v>
+      </c>
+      <c r="C117">
+        <v>10</v>
+      </c>
+      <c r="D117">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="2">
+        <v>44367.75</v>
+      </c>
+      <c r="B118">
+        <v>10</v>
+      </c>
+      <c r="C118">
+        <v>10</v>
+      </c>
+      <c r="D118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="2">
+        <v>44367.791666666657</v>
+      </c>
+      <c r="B119">
+        <v>10</v>
+      </c>
+      <c r="C119">
+        <v>10</v>
+      </c>
+      <c r="D119">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="2">
+        <v>44367.833333333343</v>
+      </c>
+      <c r="B120">
+        <v>10</v>
+      </c>
+      <c r="C120">
+        <v>10</v>
+      </c>
+      <c r="D120">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A121" s="2">
+        <v>44367.875</v>
+      </c>
+      <c r="B121">
+        <v>10</v>
+      </c>
+      <c r="C121">
+        <v>10</v>
+      </c>
+      <c r="D121">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="2">
+        <v>44367.916666666657</v>
+      </c>
+      <c r="B122">
+        <v>10</v>
+      </c>
+      <c r="C122">
+        <v>10</v>
+      </c>
+      <c r="D122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="2">
+        <v>44367.958333333343</v>
+      </c>
+      <c r="B123">
+        <v>10</v>
+      </c>
+      <c r="C123">
+        <v>10</v>
+      </c>
+      <c r="D123">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="2">
+        <v>44368</v>
+      </c>
+      <c r="B124">
+        <v>10</v>
+      </c>
+      <c r="C124">
+        <v>10</v>
+      </c>
+      <c r="D124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="2">
+        <v>44368.041666666657</v>
+      </c>
+      <c r="B125">
+        <v>10</v>
+      </c>
+      <c r="C125">
+        <v>10</v>
+      </c>
+      <c r="D125">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="2">
+        <v>44368.083333333343</v>
+      </c>
+      <c r="B126">
+        <v>10</v>
+      </c>
+      <c r="C126">
+        <v>10</v>
+      </c>
+      <c r="D126">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="2">
+        <v>44368.125</v>
+      </c>
+      <c r="B127">
+        <v>10</v>
+      </c>
+      <c r="C127">
+        <v>10</v>
+      </c>
+      <c r="D127">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="2">
+        <v>44368.166666666657</v>
+      </c>
+      <c r="B128">
+        <v>10</v>
+      </c>
+      <c r="C128">
+        <v>10</v>
+      </c>
+      <c r="D128">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="2">
+        <v>44368.208333333343</v>
+      </c>
+      <c r="B129">
+        <v>10</v>
+      </c>
+      <c r="C129">
+        <v>10</v>
+      </c>
+      <c r="D129">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="2">
+        <v>44368.25</v>
+      </c>
+      <c r="B130">
+        <v>10</v>
+      </c>
+      <c r="C130">
+        <v>10</v>
+      </c>
+      <c r="D130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="2">
+        <v>44368.291666666657</v>
+      </c>
+      <c r="B131">
+        <v>10</v>
+      </c>
+      <c r="C131">
+        <v>10</v>
+      </c>
+      <c r="D131">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A132" s="2">
+        <v>44368.333333333343</v>
+      </c>
+      <c r="B132">
+        <v>10</v>
+      </c>
+      <c r="C132">
+        <v>10</v>
+      </c>
+      <c r="D132">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="2">
+        <v>44368.375</v>
+      </c>
+      <c r="B133">
+        <v>10</v>
+      </c>
+      <c r="C133">
+        <v>10</v>
+      </c>
+      <c r="D133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="2">
+        <v>44368.416666666657</v>
+      </c>
+      <c r="B134">
+        <v>10</v>
+      </c>
+      <c r="C134">
+        <v>10</v>
+      </c>
+      <c r="D134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="2">
+        <v>44368.458333333343</v>
+      </c>
+      <c r="B135">
+        <v>10</v>
+      </c>
+      <c r="C135">
+        <v>10</v>
+      </c>
+      <c r="D135">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="2">
+        <v>44368.5</v>
+      </c>
+      <c r="B136">
+        <v>10</v>
+      </c>
+      <c r="C136">
+        <v>10</v>
+      </c>
+      <c r="D136">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="2">
+        <v>44368.541666666657</v>
+      </c>
+      <c r="B137">
+        <v>10</v>
+      </c>
+      <c r="C137">
+        <v>10</v>
+      </c>
+      <c r="D137">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="2">
+        <v>44368.583333333343</v>
+      </c>
+      <c r="B138">
+        <v>10</v>
+      </c>
+      <c r="C138">
+        <v>10</v>
+      </c>
+      <c r="D138">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="2">
+        <v>44368.625</v>
+      </c>
+      <c r="B139">
+        <v>10</v>
+      </c>
+      <c r="C139">
+        <v>10</v>
+      </c>
+      <c r="D139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="2">
+        <v>44368.666666666657</v>
+      </c>
+      <c r="B140">
+        <v>10</v>
+      </c>
+      <c r="C140">
+        <v>10</v>
+      </c>
+      <c r="D140">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="2">
+        <v>44368.708333333343</v>
+      </c>
+      <c r="B141">
+        <v>10</v>
+      </c>
+      <c r="C141">
+        <v>10</v>
+      </c>
+      <c r="D141">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="2">
+        <v>44368.75</v>
+      </c>
+      <c r="B142">
+        <v>10</v>
+      </c>
+      <c r="C142">
+        <v>10</v>
+      </c>
+      <c r="D142">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A143" s="2">
+        <v>44368.791666666657</v>
+      </c>
+      <c r="B143">
+        <v>10</v>
+      </c>
+      <c r="C143">
+        <v>10</v>
+      </c>
+      <c r="D143">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="2">
+        <v>44368.833333333343</v>
+      </c>
+      <c r="B144">
+        <v>10</v>
+      </c>
+      <c r="C144">
+        <v>10</v>
+      </c>
+      <c r="D144">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="2">
+        <v>44368.875</v>
+      </c>
+      <c r="B145">
+        <v>10</v>
+      </c>
+      <c r="C145">
+        <v>10</v>
+      </c>
+      <c r="D145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="2">
+        <v>44368.916666666657</v>
+      </c>
+      <c r="B146">
+        <v>10</v>
+      </c>
+      <c r="C146">
+        <v>10</v>
+      </c>
+      <c r="D146">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="2">
+        <v>44368.958333333343</v>
+      </c>
+      <c r="B147">
+        <v>10</v>
+      </c>
+      <c r="C147">
+        <v>10</v>
+      </c>
+      <c r="D147">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="2">
+        <v>44369</v>
+      </c>
+      <c r="B148">
+        <v>10</v>
+      </c>
+      <c r="C148">
+        <v>10</v>
+      </c>
+      <c r="D148">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="2">
+        <v>44369.041666666657</v>
+      </c>
+      <c r="B149">
+        <v>10</v>
+      </c>
+      <c r="C149">
+        <v>10</v>
+      </c>
+      <c r="D149">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="2">
+        <v>44369.083333333343</v>
+      </c>
+      <c r="B150">
+        <v>10</v>
+      </c>
+      <c r="C150">
+        <v>10</v>
+      </c>
+      <c r="D150">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="2">
+        <v>44369.125</v>
+      </c>
+      <c r="B151">
+        <v>10</v>
+      </c>
+      <c r="C151">
+        <v>10</v>
+      </c>
+      <c r="D151">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="2">
+        <v>44369.166666666657</v>
+      </c>
+      <c r="B152">
+        <v>10</v>
+      </c>
+      <c r="C152">
+        <v>10</v>
+      </c>
+      <c r="D152">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="2">
+        <v>44369.208333333343</v>
+      </c>
+      <c r="B153">
+        <v>10</v>
+      </c>
+      <c r="C153">
+        <v>10</v>
+      </c>
+      <c r="D153">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A154" s="2">
+        <v>44369.25</v>
+      </c>
+      <c r="B154">
+        <v>10</v>
+      </c>
+      <c r="C154">
+        <v>10</v>
+      </c>
+      <c r="D154">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="2">
+        <v>44369.291666666657</v>
+      </c>
+      <c r="B155">
+        <v>10</v>
+      </c>
+      <c r="C155">
+        <v>10</v>
+      </c>
+      <c r="D155">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="2">
+        <v>44369.333333333343</v>
+      </c>
+      <c r="B156">
+        <v>10</v>
+      </c>
+      <c r="C156">
+        <v>10</v>
+      </c>
+      <c r="D156">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="2">
+        <v>44369.375</v>
+      </c>
+      <c r="B157">
+        <v>10</v>
+      </c>
+      <c r="C157">
+        <v>10</v>
+      </c>
+      <c r="D157">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="2">
+        <v>44369.416666666657</v>
+      </c>
+      <c r="B158">
+        <v>10</v>
+      </c>
+      <c r="C158">
+        <v>10</v>
+      </c>
+      <c r="D158">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" s="2">
+        <v>44369.458333333343</v>
+      </c>
+      <c r="B159">
+        <v>10</v>
+      </c>
+      <c r="C159">
+        <v>10</v>
+      </c>
+      <c r="D159">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" s="2">
+        <v>44369.5</v>
+      </c>
+      <c r="B160">
+        <v>10</v>
+      </c>
+      <c r="C160">
+        <v>10</v>
+      </c>
+      <c r="D160">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="2">
+        <v>44369.541666666657</v>
+      </c>
+      <c r="B161">
+        <v>10</v>
+      </c>
+      <c r="C161">
+        <v>10</v>
+      </c>
+      <c r="D161">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="2">
+        <v>44369.583333333343</v>
+      </c>
+      <c r="B162">
+        <v>10</v>
+      </c>
+      <c r="C162">
+        <v>10</v>
+      </c>
+      <c r="D162">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="2">
+        <v>44369.625</v>
+      </c>
+      <c r="B163">
+        <v>10</v>
+      </c>
+      <c r="C163">
+        <v>10</v>
+      </c>
+      <c r="D163">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="2">
+        <v>44369.666666666657</v>
+      </c>
+      <c r="B164">
+        <v>10</v>
+      </c>
+      <c r="C164">
+        <v>10</v>
+      </c>
+      <c r="D164">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A165" s="2">
+        <v>44369.708333333343</v>
+      </c>
+      <c r="B165">
+        <v>10</v>
+      </c>
+      <c r="C165">
+        <v>10</v>
+      </c>
+      <c r="D165">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A166" s="2">
+        <v>44369.75</v>
+      </c>
+      <c r="B166">
+        <v>10</v>
+      </c>
+      <c r="C166">
+        <v>10</v>
+      </c>
+      <c r="D166">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A167" s="2">
+        <v>44369.791666666657</v>
+      </c>
+      <c r="B167">
+        <v>10</v>
+      </c>
+      <c r="C167">
+        <v>10</v>
+      </c>
+      <c r="D167">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A168" s="2">
+        <v>44369.833333333343</v>
+      </c>
+      <c r="B168">
+        <v>10</v>
+      </c>
+      <c r="C168">
+        <v>10</v>
+      </c>
+      <c r="D168">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A169" s="2">
+        <v>44369.875</v>
+      </c>
+      <c r="B169">
+        <v>10</v>
+      </c>
+      <c r="C169">
+        <v>10</v>
+      </c>
+      <c r="D169">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A170" s="2">
+        <v>44369.916666666657</v>
+      </c>
+      <c r="B170">
+        <v>10</v>
+      </c>
+      <c r="C170">
+        <v>10</v>
+      </c>
+      <c r="D170">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A171" s="2">
+        <v>44369.958333333343</v>
+      </c>
+      <c r="B171">
+        <v>10</v>
+      </c>
+      <c r="C171">
+        <v>10</v>
+      </c>
+      <c r="D171">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A172" s="2">
+        <v>44370</v>
+      </c>
+      <c r="B172">
+        <v>10</v>
+      </c>
+      <c r="C172">
+        <v>10</v>
+      </c>
+      <c r="D172">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A173" s="2">
+        <v>44370.041666666657</v>
+      </c>
+      <c r="B173">
+        <v>10</v>
+      </c>
+      <c r="C173">
+        <v>10</v>
+      </c>
+      <c r="D173">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A174" s="2">
+        <v>44370.083333333343</v>
+      </c>
+      <c r="B174">
+        <v>10</v>
+      </c>
+      <c r="C174">
+        <v>10</v>
+      </c>
+      <c r="D174">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A175" s="2">
+        <v>44370.125</v>
+      </c>
+      <c r="B175">
+        <v>10</v>
+      </c>
+      <c r="C175">
+        <v>10</v>
+      </c>
+      <c r="D175">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A176" s="2">
+        <v>44370.166666666657</v>
+      </c>
+      <c r="B176">
+        <v>10</v>
+      </c>
+      <c r="C176">
+        <v>10</v>
+      </c>
+      <c r="D176">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A177" s="2">
+        <v>44370.208333333343</v>
+      </c>
+      <c r="B177">
+        <v>10</v>
+      </c>
+      <c r="C177">
+        <v>10</v>
+      </c>
+      <c r="D177">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A178" s="2">
+        <v>44370.25</v>
+      </c>
+      <c r="B178">
+        <v>10</v>
+      </c>
+      <c r="C178">
+        <v>10</v>
+      </c>
+      <c r="D178">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A179" s="2">
+        <v>44370.291666666657</v>
+      </c>
+      <c r="B179">
+        <v>10</v>
+      </c>
+      <c r="C179">
+        <v>10</v>
+      </c>
+      <c r="D179">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A180" s="2">
+        <v>44370.333333333343</v>
+      </c>
+      <c r="B180">
+        <v>10</v>
+      </c>
+      <c r="C180">
+        <v>10</v>
+      </c>
+      <c r="D180">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A181" s="2">
+        <v>44370.375</v>
+      </c>
+      <c r="B181">
+        <v>10</v>
+      </c>
+      <c r="C181">
+        <v>10</v>
+      </c>
+      <c r="D181">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A182" s="2">
+        <v>44370.416666666657</v>
+      </c>
+      <c r="B182">
+        <v>10</v>
+      </c>
+      <c r="C182">
+        <v>10</v>
+      </c>
+      <c r="D182">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A183" s="2">
+        <v>44370.458333333343</v>
+      </c>
+      <c r="B183">
+        <v>10</v>
+      </c>
+      <c r="C183">
+        <v>10</v>
+      </c>
+      <c r="D183">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A184" s="2">
+        <v>44370.5</v>
+      </c>
+      <c r="B184">
+        <v>10</v>
+      </c>
+      <c r="C184">
+        <v>10</v>
+      </c>
+      <c r="D184">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="2">
+        <v>44370.541666666657</v>
+      </c>
+      <c r="B185">
+        <v>10</v>
+      </c>
+      <c r="C185">
+        <v>10</v>
+      </c>
+      <c r="D185">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="2">
+        <v>44370.583333333343</v>
+      </c>
+      <c r="B186">
+        <v>10</v>
+      </c>
+      <c r="C186">
+        <v>10</v>
+      </c>
+      <c r="D186">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A187" s="2">
+        <v>44370.625</v>
+      </c>
+      <c r="B187">
+        <v>10</v>
+      </c>
+      <c r="C187">
+        <v>10</v>
+      </c>
+      <c r="D187">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A188" s="2">
+        <v>44370.666666666657</v>
+      </c>
+      <c r="B188">
+        <v>10</v>
+      </c>
+      <c r="C188">
+        <v>10</v>
+      </c>
+      <c r="D188">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A189" s="2">
+        <v>44370.708333333343</v>
+      </c>
+      <c r="B189">
+        <v>10</v>
+      </c>
+      <c r="C189">
+        <v>10</v>
+      </c>
+      <c r="D189">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A190" s="2">
+        <v>44370.75</v>
+      </c>
+      <c r="B190">
+        <v>10</v>
+      </c>
+      <c r="C190">
+        <v>10</v>
+      </c>
+      <c r="D190">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A191" s="2">
+        <v>44370.791666666657</v>
+      </c>
+      <c r="B191">
+        <v>10</v>
+      </c>
+      <c r="C191">
+        <v>10</v>
+      </c>
+      <c r="D191">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A192" s="2">
+        <v>44370.833333333343</v>
+      </c>
+      <c r="B192">
+        <v>10</v>
+      </c>
+      <c r="C192">
+        <v>10</v>
+      </c>
+      <c r="D192">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A193" s="2">
+        <v>44370.875</v>
+      </c>
+      <c r="B193">
+        <v>10</v>
+      </c>
+      <c r="C193">
+        <v>10</v>
+      </c>
+      <c r="D193">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A194" s="2">
+        <v>44370.916666666657</v>
+      </c>
+      <c r="B194">
+        <v>10</v>
+      </c>
+      <c r="C194">
+        <v>10</v>
+      </c>
+      <c r="D194">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A195" s="2">
+        <v>44370.958333333343</v>
+      </c>
+      <c r="B195">
+        <v>10</v>
+      </c>
+      <c r="C195">
+        <v>10</v>
+      </c>
+      <c r="D195">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A196" s="2">
+        <v>44371</v>
+      </c>
+      <c r="B196">
+        <v>10</v>
+      </c>
+      <c r="C196">
+        <v>10</v>
+      </c>
+      <c r="D196">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A197" s="2">
+        <v>44371.041666666657</v>
+      </c>
+      <c r="B197">
+        <v>10</v>
+      </c>
+      <c r="C197">
+        <v>10</v>
+      </c>
+      <c r="D197">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A198" s="2">
+        <v>44371.083333333343</v>
+      </c>
+      <c r="B198">
+        <v>10</v>
+      </c>
+      <c r="C198">
+        <v>10</v>
+      </c>
+      <c r="D198">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A199" s="2">
+        <v>44371.125</v>
+      </c>
+      <c r="B199">
+        <v>10</v>
+      </c>
+      <c r="C199">
+        <v>10</v>
+      </c>
+      <c r="D199">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A200" s="2">
+        <v>44371.166666666657</v>
+      </c>
+      <c r="B200">
+        <v>10</v>
+      </c>
+      <c r="C200">
+        <v>10</v>
+      </c>
+      <c r="D200">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A201" s="2">
+        <v>44371.208333333343</v>
+      </c>
+      <c r="B201">
+        <v>10</v>
+      </c>
+      <c r="C201">
+        <v>10</v>
+      </c>
+      <c r="D201">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A202" s="2">
+        <v>44371.25</v>
+      </c>
+      <c r="B202">
+        <v>10</v>
+      </c>
+      <c r="C202">
+        <v>10</v>
+      </c>
+      <c r="D202">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A203" s="2">
+        <v>44371.291666666657</v>
+      </c>
+      <c r="B203">
+        <v>10</v>
+      </c>
+      <c r="C203">
+        <v>10</v>
+      </c>
+      <c r="D203">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A204" s="2">
+        <v>44371.333333333343</v>
+      </c>
+      <c r="B204">
+        <v>10</v>
+      </c>
+      <c r="C204">
+        <v>10</v>
+      </c>
+      <c r="D204">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A205" s="2">
+        <v>44371.375</v>
+      </c>
+      <c r="B205">
+        <v>10</v>
+      </c>
+      <c r="C205">
+        <v>10</v>
+      </c>
+      <c r="D205">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A206" s="2">
+        <v>44371.416666666657</v>
+      </c>
+      <c r="B206">
+        <v>10</v>
+      </c>
+      <c r="C206">
+        <v>10</v>
+      </c>
+      <c r="D206">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A207" s="2">
+        <v>44371.458333333343</v>
+      </c>
+      <c r="B207">
+        <v>10</v>
+      </c>
+      <c r="C207">
+        <v>10</v>
+      </c>
+      <c r="D207">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A208" s="2">
+        <v>44371.5</v>
+      </c>
+      <c r="B208">
+        <v>10</v>
+      </c>
+      <c r="C208">
+        <v>10</v>
+      </c>
+      <c r="D208">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A209" s="2">
+        <v>44371.541666666657</v>
+      </c>
+      <c r="B209">
+        <v>10</v>
+      </c>
+      <c r="C209">
+        <v>10</v>
+      </c>
+      <c r="D209">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A210" s="2">
+        <v>44371.583333333343</v>
+      </c>
+      <c r="B210">
+        <v>10</v>
+      </c>
+      <c r="C210">
+        <v>10</v>
+      </c>
+      <c r="D210">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A211" s="2">
+        <v>44371.625</v>
+      </c>
+      <c r="B211">
+        <v>10</v>
+      </c>
+      <c r="C211">
+        <v>10</v>
+      </c>
+      <c r="D211">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A212" s="2">
+        <v>44371.666666666657</v>
+      </c>
+      <c r="B212">
+        <v>10</v>
+      </c>
+      <c r="C212">
+        <v>10</v>
+      </c>
+      <c r="D212">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A213" s="2">
+        <v>44371.708333333343</v>
+      </c>
+      <c r="B213">
+        <v>10</v>
+      </c>
+      <c r="C213">
+        <v>10</v>
+      </c>
+      <c r="D213">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A214" s="2">
+        <v>44371.75</v>
+      </c>
+      <c r="B214">
+        <v>10</v>
+      </c>
+      <c r="C214">
+        <v>10</v>
+      </c>
+      <c r="D214">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A215" s="2">
+        <v>44371.791666666657</v>
+      </c>
+      <c r="B215">
+        <v>10</v>
+      </c>
+      <c r="C215">
+        <v>10</v>
+      </c>
+      <c r="D215">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A216" s="2">
+        <v>44371.833333333343</v>
+      </c>
+      <c r="B216">
+        <v>10</v>
+      </c>
+      <c r="C216">
+        <v>10</v>
+      </c>
+      <c r="D216">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A217" s="2">
+        <v>44371.875</v>
+      </c>
+      <c r="B217">
+        <v>10</v>
+      </c>
+      <c r="C217">
+        <v>10</v>
+      </c>
+      <c r="D217">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A218" s="2">
+        <v>44371.916666666657</v>
+      </c>
+      <c r="B218">
+        <v>10</v>
+      </c>
+      <c r="C218">
+        <v>10</v>
+      </c>
+      <c r="D218">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A219" s="2">
+        <v>44371.958333333343</v>
+      </c>
+      <c r="B219">
+        <v>10</v>
+      </c>
+      <c r="C219">
+        <v>10</v>
+      </c>
+      <c r="D219">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A220" s="2">
+        <v>44372</v>
+      </c>
+      <c r="B220">
+        <v>10</v>
+      </c>
+      <c r="C220">
+        <v>10</v>
+      </c>
+      <c r="D220">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A221" s="2">
+        <v>44372.041666666657</v>
+      </c>
+      <c r="B221">
+        <v>10</v>
+      </c>
+      <c r="C221">
+        <v>10</v>
+      </c>
+      <c r="D221">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A222" s="2">
+        <v>44372.083333333343</v>
+      </c>
+      <c r="B222">
+        <v>10</v>
+      </c>
+      <c r="C222">
+        <v>10</v>
+      </c>
+      <c r="D222">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A223" s="2">
+        <v>44372.125</v>
+      </c>
+      <c r="B223">
+        <v>10</v>
+      </c>
+      <c r="C223">
+        <v>10</v>
+      </c>
+      <c r="D223">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A224" s="2">
+        <v>44372.166666666657</v>
+      </c>
+      <c r="B224">
+        <v>10</v>
+      </c>
+      <c r="C224">
+        <v>10</v>
+      </c>
+      <c r="D224">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A225" s="2">
+        <v>44372.208333333343</v>
+      </c>
+      <c r="B225">
+        <v>10</v>
+      </c>
+      <c r="C225">
+        <v>10</v>
+      </c>
+      <c r="D225">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A226" s="2">
+        <v>44372.25</v>
+      </c>
+      <c r="B226">
+        <v>10</v>
+      </c>
+      <c r="C226">
+        <v>10</v>
+      </c>
+      <c r="D226">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A227" s="2">
+        <v>44372.291666666657</v>
+      </c>
+      <c r="B227">
+        <v>10</v>
+      </c>
+      <c r="C227">
+        <v>10</v>
+      </c>
+      <c r="D227">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A228" s="2">
+        <v>44372.333333333343</v>
+      </c>
+      <c r="B228">
+        <v>10</v>
+      </c>
+      <c r="C228">
+        <v>10</v>
+      </c>
+      <c r="D228">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A229" s="2">
+        <v>44372.375</v>
+      </c>
+      <c r="B229">
+        <v>10</v>
+      </c>
+      <c r="C229">
+        <v>10</v>
+      </c>
+      <c r="D229">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A230" s="2">
+        <v>44372.416666666657</v>
+      </c>
+      <c r="B230">
+        <v>10</v>
+      </c>
+      <c r="C230">
+        <v>10</v>
+      </c>
+      <c r="D230">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A231" s="2">
+        <v>44372.458333333343</v>
+      </c>
+      <c r="B231">
+        <v>10</v>
+      </c>
+      <c r="C231">
+        <v>10</v>
+      </c>
+      <c r="D231">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A232" s="2">
+        <v>44372.5</v>
+      </c>
+      <c r="B232">
+        <v>10</v>
+      </c>
+      <c r="C232">
+        <v>10</v>
+      </c>
+      <c r="D232">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A233" s="2">
+        <v>44372.541666666657</v>
+      </c>
+      <c r="B233">
+        <v>10</v>
+      </c>
+      <c r="C233">
+        <v>10</v>
+      </c>
+      <c r="D233">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A234" s="2">
+        <v>44372.583333333343</v>
+      </c>
+      <c r="B234">
+        <v>10</v>
+      </c>
+      <c r="C234">
+        <v>10</v>
+      </c>
+      <c r="D234">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A235" s="2">
+        <v>44372.625</v>
+      </c>
+      <c r="B235">
+        <v>10</v>
+      </c>
+      <c r="C235">
+        <v>10</v>
+      </c>
+      <c r="D235">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A236" s="2">
+        <v>44372.666666666657</v>
+      </c>
+      <c r="B236">
+        <v>10</v>
+      </c>
+      <c r="C236">
+        <v>10</v>
+      </c>
+      <c r="D236">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A237" s="2">
+        <v>44372.708333333343</v>
+      </c>
+      <c r="B237">
+        <v>10</v>
+      </c>
+      <c r="C237">
+        <v>10</v>
+      </c>
+      <c r="D237">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A238" s="2">
+        <v>44372.75</v>
+      </c>
+      <c r="B238">
+        <v>10</v>
+      </c>
+      <c r="C238">
+        <v>10</v>
+      </c>
+      <c r="D238">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A239" s="2">
+        <v>44372.791666666657</v>
+      </c>
+      <c r="B239">
+        <v>10</v>
+      </c>
+      <c r="C239">
+        <v>10</v>
+      </c>
+      <c r="D239">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A240" s="2">
+        <v>44372.833333333343</v>
+      </c>
+      <c r="B240">
+        <v>10</v>
+      </c>
+      <c r="C240">
+        <v>10</v>
+      </c>
+      <c r="D240">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A241" s="2">
+        <v>44372.875</v>
+      </c>
+      <c r="B241">
+        <v>10</v>
+      </c>
+      <c r="C241">
+        <v>10</v>
+      </c>
+      <c r="D241">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A242" s="2">
+        <v>44372.916666666657</v>
+      </c>
+      <c r="B242">
+        <v>10</v>
+      </c>
+      <c r="C242">
+        <v>10</v>
+      </c>
+      <c r="D242">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A243" s="2">
+        <v>44372.958333333343</v>
+      </c>
+      <c r="B243">
+        <v>10</v>
+      </c>
+      <c r="C243">
+        <v>10</v>
+      </c>
+      <c r="D243">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A244" s="2">
+        <v>44373</v>
+      </c>
+      <c r="B244">
+        <v>10</v>
+      </c>
+      <c r="C244">
+        <v>10</v>
+      </c>
+      <c r="D244">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A245" s="2">
+        <v>44373.041666666657</v>
+      </c>
+      <c r="B245">
+        <v>10</v>
+      </c>
+      <c r="C245">
+        <v>10</v>
+      </c>
+      <c r="D245">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A246" s="2">
+        <v>44373.083333333343</v>
+      </c>
+      <c r="B246">
+        <v>10</v>
+      </c>
+      <c r="C246">
+        <v>10</v>
+      </c>
+      <c r="D246">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A247" s="2">
+        <v>44373.125</v>
+      </c>
+      <c r="B247">
+        <v>10</v>
+      </c>
+      <c r="C247">
+        <v>10</v>
+      </c>
+      <c r="D247">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A248" s="2">
+        <v>44373.166666666657</v>
+      </c>
+      <c r="B248">
+        <v>10</v>
+      </c>
+      <c r="C248">
+        <v>10</v>
+      </c>
+      <c r="D248">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="249" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A249" s="2">
+        <v>44373.208333333343</v>
+      </c>
+      <c r="B249">
+        <v>10</v>
+      </c>
+      <c r="C249">
+        <v>10</v>
+      </c>
+      <c r="D249">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A250" s="2">
+        <v>44373.25</v>
+      </c>
+      <c r="B250">
+        <v>10</v>
+      </c>
+      <c r="C250">
+        <v>10</v>
+      </c>
+      <c r="D250">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A251" s="2">
+        <v>44373.291666666657</v>
+      </c>
+      <c r="B251">
+        <v>10</v>
+      </c>
+      <c r="C251">
+        <v>10</v>
+      </c>
+      <c r="D251">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A252" s="2">
+        <v>44373.333333333343</v>
+      </c>
+      <c r="B252">
+        <v>10</v>
+      </c>
+      <c r="C252">
+        <v>10</v>
+      </c>
+      <c r="D252">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A253" s="2">
+        <v>44373.375</v>
+      </c>
+      <c r="B253">
+        <v>10</v>
+      </c>
+      <c r="C253">
+        <v>10</v>
+      </c>
+      <c r="D253">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A254" s="2">
+        <v>44373.416666666657</v>
+      </c>
+      <c r="B254">
+        <v>10</v>
+      </c>
+      <c r="C254">
+        <v>10</v>
+      </c>
+      <c r="D254">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A255" s="2">
+        <v>44373.458333333343</v>
+      </c>
+      <c r="B255">
+        <v>10</v>
+      </c>
+      <c r="C255">
+        <v>10</v>
+      </c>
+      <c r="D255">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A256" s="2">
+        <v>44373.5</v>
+      </c>
+      <c r="B256">
+        <v>10</v>
+      </c>
+      <c r="C256">
+        <v>10</v>
+      </c>
+      <c r="D256">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A257" s="2">
+        <v>44373.541666666657</v>
+      </c>
+      <c r="B257">
+        <v>10</v>
+      </c>
+      <c r="C257">
+        <v>10</v>
+      </c>
+      <c r="D257">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A258" s="2">
+        <v>44373.583333333343</v>
+      </c>
+      <c r="B258">
+        <v>10</v>
+      </c>
+      <c r="C258">
+        <v>10</v>
+      </c>
+      <c r="D258">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A259" s="2">
+        <v>44373.625</v>
+      </c>
+      <c r="B259">
+        <v>10</v>
+      </c>
+      <c r="C259">
+        <v>10</v>
+      </c>
+      <c r="D259">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A260" s="2">
+        <v>44373.666666666657</v>
+      </c>
+      <c r="B260">
+        <v>10</v>
+      </c>
+      <c r="C260">
+        <v>10</v>
+      </c>
+      <c r="D260">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A261" s="2">
+        <v>44373.708333333343</v>
+      </c>
+      <c r="B261">
+        <v>10</v>
+      </c>
+      <c r="C261">
+        <v>10</v>
+      </c>
+      <c r="D261">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A262" s="2">
+        <v>44373.75</v>
+      </c>
+      <c r="B262">
+        <v>10</v>
+      </c>
+      <c r="C262">
+        <v>10</v>
+      </c>
+      <c r="D262">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A263" s="2">
+        <v>44373.791666666657</v>
+      </c>
+      <c r="B263">
+        <v>10</v>
+      </c>
+      <c r="C263">
+        <v>10</v>
+      </c>
+      <c r="D263">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A264" s="2">
+        <v>44373.833333333343</v>
+      </c>
+      <c r="B264">
+        <v>10</v>
+      </c>
+      <c r="C264">
+        <v>10</v>
+      </c>
+      <c r="D264">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A265" s="2">
+        <v>44373.875</v>
+      </c>
+      <c r="B265">
+        <v>10</v>
+      </c>
+      <c r="C265">
+        <v>10</v>
+      </c>
+      <c r="D265">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A266" s="2">
+        <v>44373.916666666657</v>
+      </c>
+      <c r="B266">
+        <v>10</v>
+      </c>
+      <c r="C266">
+        <v>10</v>
+      </c>
+      <c r="D266">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A267" s="2">
+        <v>44373.958333333343</v>
+      </c>
+      <c r="B267">
+        <v>10</v>
+      </c>
+      <c r="C267">
+        <v>10</v>
+      </c>
+      <c r="D267">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="268" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A268" s="2">
+        <v>44374</v>
+      </c>
+      <c r="B268">
+        <v>10</v>
+      </c>
+      <c r="C268">
+        <v>10</v>
+      </c>
+      <c r="D268">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="269" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A269" s="2">
+        <v>44374.041666666657</v>
+      </c>
+      <c r="B269">
+        <v>10</v>
+      </c>
+      <c r="C269">
+        <v>10</v>
+      </c>
+      <c r="D269">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="270" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A270" s="2">
+        <v>44374.083333333343</v>
+      </c>
+      <c r="B270">
+        <v>10</v>
+      </c>
+      <c r="C270">
+        <v>10</v>
+      </c>
+      <c r="D270">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="271" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A271" s="2">
+        <v>44374.125</v>
+      </c>
+      <c r="B271">
+        <v>10</v>
+      </c>
+      <c r="C271">
+        <v>10</v>
+      </c>
+      <c r="D271">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="272" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A272" s="2">
+        <v>44374.166666666657</v>
+      </c>
+      <c r="B272">
+        <v>10</v>
+      </c>
+      <c r="C272">
+        <v>10</v>
+      </c>
+      <c r="D272">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="273" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A273" s="2">
+        <v>44374.208333333343</v>
+      </c>
+      <c r="B273">
+        <v>10</v>
+      </c>
+      <c r="C273">
+        <v>10</v>
+      </c>
+      <c r="D273">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="274" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A274" s="2">
+        <v>44374.25</v>
+      </c>
+      <c r="B274">
+        <v>10</v>
+      </c>
+      <c r="C274">
+        <v>10</v>
+      </c>
+      <c r="D274">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="275" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A275" s="2">
+        <v>44374.291666666657</v>
+      </c>
+      <c r="B275">
+        <v>10</v>
+      </c>
+      <c r="C275">
+        <v>10</v>
+      </c>
+      <c r="D275">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="276" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A276" s="2">
+        <v>44374.333333333343</v>
+      </c>
+      <c r="B276">
+        <v>10</v>
+      </c>
+      <c r="C276">
+        <v>10</v>
+      </c>
+      <c r="D276">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="277" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A277" s="2">
+        <v>44374.375</v>
+      </c>
+      <c r="B277">
+        <v>10</v>
+      </c>
+      <c r="C277">
+        <v>10</v>
+      </c>
+      <c r="D277">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A278" s="2">
+        <v>44374.416666666657</v>
+      </c>
+      <c r="B278">
+        <v>10</v>
+      </c>
+      <c r="C278">
+        <v>10</v>
+      </c>
+      <c r="D278">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A279" s="2">
+        <v>44374.458333333343</v>
+      </c>
+      <c r="B279">
+        <v>10</v>
+      </c>
+      <c r="C279">
+        <v>10</v>
+      </c>
+      <c r="D279">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A280" s="2">
+        <v>44374.5</v>
+      </c>
+      <c r="B280">
+        <v>10</v>
+      </c>
+      <c r="C280">
+        <v>10</v>
+      </c>
+      <c r="D280">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="281" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A281" s="2">
+        <v>44374.541666666657</v>
+      </c>
+      <c r="B281">
+        <v>10</v>
+      </c>
+      <c r="C281">
+        <v>10</v>
+      </c>
+      <c r="D281">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="282" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A282" s="2">
+        <v>44374.583333333343</v>
+      </c>
+      <c r="B282">
+        <v>10</v>
+      </c>
+      <c r="C282">
+        <v>10</v>
+      </c>
+      <c r="D282">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="283" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A283" s="2">
+        <v>44374.625</v>
+      </c>
+      <c r="B283">
+        <v>10</v>
+      </c>
+      <c r="C283">
+        <v>10</v>
+      </c>
+      <c r="D283">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="284" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A284" s="2">
+        <v>44374.666666666657</v>
+      </c>
+      <c r="B284">
+        <v>10</v>
+      </c>
+      <c r="C284">
+        <v>10</v>
+      </c>
+      <c r="D284">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="285" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A285" s="2">
+        <v>44374.708333333343</v>
+      </c>
+      <c r="B285">
+        <v>10</v>
+      </c>
+      <c r="C285">
+        <v>10</v>
+      </c>
+      <c r="D285">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A286" s="2">
+        <v>44374.75</v>
+      </c>
+      <c r="B286">
+        <v>10</v>
+      </c>
+      <c r="C286">
+        <v>10</v>
+      </c>
+      <c r="D286">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="287" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A287" s="2">
+        <v>44374.791666666657</v>
+      </c>
+      <c r="B287">
+        <v>10</v>
+      </c>
+      <c r="C287">
+        <v>10</v>
+      </c>
+      <c r="D287">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A288" s="2">
+        <v>44374.833333333343</v>
+      </c>
+      <c r="B288">
+        <v>10</v>
+      </c>
+      <c r="C288">
+        <v>10</v>
+      </c>
+      <c r="D288">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A289" s="2">
+        <v>44374.875</v>
+      </c>
+      <c r="B289">
+        <v>10</v>
+      </c>
+      <c r="C289">
+        <v>10</v>
+      </c>
+      <c r="D289">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="290" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A290" s="2">
+        <v>44374.916666666657</v>
+      </c>
+      <c r="B290">
+        <v>10</v>
+      </c>
+      <c r="C290">
+        <v>10</v>
+      </c>
+      <c r="D290">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="291" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A291" s="2">
+        <v>44374.958333333343</v>
+      </c>
+      <c r="B291">
+        <v>10</v>
+      </c>
+      <c r="C291">
+        <v>10</v>
+      </c>
+      <c r="D291">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="292" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A292" s="2">
+        <v>44375</v>
+      </c>
+      <c r="B292">
+        <v>10</v>
+      </c>
+      <c r="C292">
+        <v>10</v>
+      </c>
+      <c r="D292">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="293" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A293" s="2">
+        <v>44375.041666666657</v>
+      </c>
+      <c r="B293">
+        <v>10</v>
+      </c>
+      <c r="C293">
+        <v>10</v>
+      </c>
+      <c r="D293">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="294" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A294" s="2">
+        <v>44375.083333333343</v>
+      </c>
+      <c r="B294">
+        <v>10</v>
+      </c>
+      <c r="C294">
+        <v>10</v>
+      </c>
+      <c r="D294">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="295" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A295" s="2">
+        <v>44375.125</v>
+      </c>
+      <c r="B295">
+        <v>10</v>
+      </c>
+      <c r="C295">
+        <v>10</v>
+      </c>
+      <c r="D295">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="296" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A296" s="2">
+        <v>44375.166666666657</v>
+      </c>
+      <c r="B296">
+        <v>10</v>
+      </c>
+      <c r="C296">
+        <v>10</v>
+      </c>
+      <c r="D296">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="297" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A297" s="2">
+        <v>44375.208333333343</v>
+      </c>
+      <c r="B297">
+        <v>10</v>
+      </c>
+      <c r="C297">
+        <v>10</v>
+      </c>
+      <c r="D297">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="298" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A298" s="2">
+        <v>44375.25</v>
+      </c>
+      <c r="B298">
+        <v>10</v>
+      </c>
+      <c r="C298">
+        <v>10</v>
+      </c>
+      <c r="D298">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A299" s="2">
+        <v>44375.291666666657</v>
+      </c>
+      <c r="B299">
+        <v>10</v>
+      </c>
+      <c r="C299">
+        <v>10</v>
+      </c>
+      <c r="D299">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A300" s="2">
+        <v>44375.333333333343</v>
+      </c>
+      <c r="B300">
+        <v>10</v>
+      </c>
+      <c r="C300">
+        <v>10</v>
+      </c>
+      <c r="D300">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A301" s="2">
+        <v>44375.375</v>
+      </c>
+      <c r="B301">
+        <v>10</v>
+      </c>
+      <c r="C301">
+        <v>10</v>
+      </c>
+      <c r="D301">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="302" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A302" s="2">
+        <v>44375.416666666657</v>
+      </c>
+      <c r="B302">
+        <v>10</v>
+      </c>
+      <c r="C302">
+        <v>10</v>
+      </c>
+      <c r="D302">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="303" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A303" s="2">
+        <v>44375.458333333343</v>
+      </c>
+      <c r="B303">
+        <v>10</v>
+      </c>
+      <c r="C303">
+        <v>10</v>
+      </c>
+      <c r="D303">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="304" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A304" s="2">
+        <v>44375.5</v>
+      </c>
+      <c r="B304">
+        <v>10</v>
+      </c>
+      <c r="C304">
+        <v>10</v>
+      </c>
+      <c r="D304">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="305" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A305" s="2">
+        <v>44375.541666666657</v>
+      </c>
+      <c r="B305">
+        <v>10</v>
+      </c>
+      <c r="C305">
+        <v>10</v>
+      </c>
+      <c r="D305">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A306" s="2">
+        <v>44375.583333333343</v>
+      </c>
+      <c r="B306">
+        <v>10</v>
+      </c>
+      <c r="C306">
+        <v>10</v>
+      </c>
+      <c r="D306">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A307" s="2">
+        <v>44375.625</v>
+      </c>
+      <c r="B307">
+        <v>10</v>
+      </c>
+      <c r="C307">
+        <v>10</v>
+      </c>
+      <c r="D307">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="308" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A308" s="2">
+        <v>44375.666666666657</v>
+      </c>
+      <c r="B308">
+        <v>10</v>
+      </c>
+      <c r="C308">
+        <v>10</v>
+      </c>
+      <c r="D308">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="309" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A309" s="2">
+        <v>44375.708333333343</v>
+      </c>
+      <c r="B309">
+        <v>10</v>
+      </c>
+      <c r="C309">
+        <v>10</v>
+      </c>
+      <c r="D309">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A310" s="2">
+        <v>44375.75</v>
+      </c>
+      <c r="B310">
+        <v>10</v>
+      </c>
+      <c r="C310">
+        <v>10</v>
+      </c>
+      <c r="D310">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="311" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A311" s="2">
+        <v>44375.791666666657</v>
+      </c>
+      <c r="B311">
+        <v>10</v>
+      </c>
+      <c r="C311">
+        <v>10</v>
+      </c>
+      <c r="D311">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="312" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A312" s="2">
+        <v>44375.833333333343</v>
+      </c>
+      <c r="B312">
+        <v>10</v>
+      </c>
+      <c r="C312">
+        <v>10</v>
+      </c>
+      <c r="D312">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="313" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A313" s="2">
+        <v>44375.875</v>
+      </c>
+      <c r="B313">
+        <v>10</v>
+      </c>
+      <c r="C313">
+        <v>10</v>
+      </c>
+      <c r="D313">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="314" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A314" s="2">
+        <v>44375.916666666657</v>
+      </c>
+      <c r="B314">
+        <v>10</v>
+      </c>
+      <c r="C314">
+        <v>10</v>
+      </c>
+      <c r="D314">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="315" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A315" s="2">
+        <v>44375.958333333343</v>
+      </c>
+      <c r="B315">
+        <v>10</v>
+      </c>
+      <c r="C315">
+        <v>10</v>
+      </c>
+      <c r="D315">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A316" s="2">
+        <v>44376</v>
+      </c>
+      <c r="B316">
+        <v>10</v>
+      </c>
+      <c r="C316">
+        <v>10</v>
+      </c>
+      <c r="D316">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="317" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A317" s="2">
+        <v>44376.041666666657</v>
+      </c>
+      <c r="B317">
+        <v>10</v>
+      </c>
+      <c r="C317">
+        <v>10</v>
+      </c>
+      <c r="D317">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="318" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A318" s="2">
+        <v>44376.083333333343</v>
+      </c>
+      <c r="B318">
+        <v>10</v>
+      </c>
+      <c r="C318">
+        <v>10</v>
+      </c>
+      <c r="D318">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="319" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A319" s="2">
+        <v>44376.125</v>
+      </c>
+      <c r="B319">
+        <v>10</v>
+      </c>
+      <c r="C319">
+        <v>10</v>
+      </c>
+      <c r="D319">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A320" s="2">
+        <v>44376.166666666657</v>
+      </c>
+      <c r="B320">
+        <v>10</v>
+      </c>
+      <c r="C320">
+        <v>10</v>
+      </c>
+      <c r="D320">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A321" s="2">
+        <v>44376.208333333343</v>
+      </c>
+      <c r="B321">
+        <v>10</v>
+      </c>
+      <c r="C321">
+        <v>10</v>
+      </c>
+      <c r="D321">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="322" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A322" s="2">
+        <v>44376.25</v>
+      </c>
+      <c r="B322">
+        <v>10</v>
+      </c>
+      <c r="C322">
+        <v>10</v>
+      </c>
+      <c r="D322">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="323" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A323" s="2">
+        <v>44376.291666666657</v>
+      </c>
+      <c r="B323">
+        <v>10</v>
+      </c>
+      <c r="C323">
+        <v>10</v>
+      </c>
+      <c r="D323">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="324" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A324" s="2">
+        <v>44376.333333333343</v>
+      </c>
+      <c r="B324">
+        <v>10</v>
+      </c>
+      <c r="C324">
+        <v>10</v>
+      </c>
+      <c r="D324">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="325" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A325" s="2">
+        <v>44376.375</v>
+      </c>
+      <c r="B325">
+        <v>10</v>
+      </c>
+      <c r="C325">
+        <v>10</v>
+      </c>
+      <c r="D325">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="326" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A326" s="2">
+        <v>44376.416666666657</v>
+      </c>
+      <c r="B326">
+        <v>10</v>
+      </c>
+      <c r="C326">
+        <v>10</v>
+      </c>
+      <c r="D326">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="327" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A327" s="2">
+        <v>44376.458333333343</v>
+      </c>
+      <c r="B327">
+        <v>10</v>
+      </c>
+      <c r="C327">
+        <v>10</v>
+      </c>
+      <c r="D327">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="328" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A328" s="2">
+        <v>44376.5</v>
+      </c>
+      <c r="B328">
+        <v>10</v>
+      </c>
+      <c r="C328">
+        <v>10</v>
+      </c>
+      <c r="D328">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="329" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A329" s="2">
+        <v>44376.541666666657</v>
+      </c>
+      <c r="B329">
+        <v>10</v>
+      </c>
+      <c r="C329">
+        <v>10</v>
+      </c>
+      <c r="D329">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="330" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A330" s="2">
+        <v>44376.583333333343</v>
+      </c>
+      <c r="B330">
+        <v>10</v>
+      </c>
+      <c r="C330">
+        <v>10</v>
+      </c>
+      <c r="D330">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A331" s="2">
+        <v>44376.625</v>
+      </c>
+      <c r="B331">
+        <v>10</v>
+      </c>
+      <c r="C331">
+        <v>10</v>
+      </c>
+      <c r="D331">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A332" s="2">
+        <v>44376.666666666657</v>
+      </c>
+      <c r="B332">
+        <v>10</v>
+      </c>
+      <c r="C332">
+        <v>10</v>
+      </c>
+      <c r="D332">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A333" s="2">
+        <v>44376.708333333343</v>
+      </c>
+      <c r="B333">
+        <v>10</v>
+      </c>
+      <c r="C333">
+        <v>10</v>
+      </c>
+      <c r="D333">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A334" s="2">
+        <v>44376.75</v>
+      </c>
+      <c r="B334">
+        <v>10</v>
+      </c>
+      <c r="C334">
+        <v>10</v>
+      </c>
+      <c r="D334">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A335" s="2">
+        <v>44376.791666666657</v>
+      </c>
+      <c r="B335">
+        <v>10</v>
+      </c>
+      <c r="C335">
+        <v>10</v>
+      </c>
+      <c r="D335">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="336" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A336" s="2">
+        <v>44376.833333333343</v>
+      </c>
+      <c r="B336">
+        <v>10</v>
+      </c>
+      <c r="C336">
+        <v>10</v>
+      </c>
+      <c r="D336">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A337" s="2">
+        <v>44376.875</v>
+      </c>
+      <c r="B337">
+        <v>10</v>
+      </c>
+      <c r="C337">
+        <v>10</v>
+      </c>
+      <c r="D337">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A338" s="2">
+        <v>44376.916666666657</v>
+      </c>
+      <c r="B338">
+        <v>10</v>
+      </c>
+      <c r="C338">
+        <v>10</v>
+      </c>
+      <c r="D338">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="339" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A339" s="2">
+        <v>44376.958333333343</v>
+      </c>
+      <c r="B339">
+        <v>10</v>
+      </c>
+      <c r="C339">
+        <v>10</v>
+      </c>
+      <c r="D339">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>